<commit_message>
version of the manuscript that will be sent to Grace
</commit_message>
<xml_diff>
--- a/tables/afs-typology.xlsx
+++ b/tables/afs-typology.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\PSAFcarbonPaper\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868B91F9-5AF5-4437-8E27-1C11F83D14E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2D8E9-DC09-41E9-9005-153A723180B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>0 to 3 years</t>
   </si>
   <si>
-    <t>Sylvopastoral land (pasture, savanna or secondary forest), Forest garden</t>
-  </si>
-  <si>
     <t>Corn, peanut, sweet potatoes, cucurbitaceae, beans</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Eucalyptus alba, Timonius, Rosewood, Tamarind, Kussum tree, Ziziphus mauritiana, Albizia julibrissim, Corypha</t>
   </si>
   <si>
-    <t>Sylvopastoral (SP)</t>
-  </si>
-  <si>
     <t>Ai bobur laran, ai loek laran, tree's name-laran (inside -the place of- the main tree and/or functional tree), pastagem (pasture)</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>2 to 10 years</t>
   </si>
   <si>
-    <t>Crop system including a fallow phase,  Sylvopastoral land (pasture, savanna or secondary forest), Forest garden</t>
-  </si>
-  <si>
     <t>Chili, papaya, condiment, vegetable, banana</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>&gt; 5 years</t>
   </si>
   <si>
-    <t>Crop system including a fallow phase, Young agroforest</t>
-  </si>
-  <si>
     <t>Corn, cassava, taro, yam, vegetable, condiment, banana, bamboo, papaya cucurbitaceae, beans, chili.</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>Close to a stream (can be dry during the dry season)</t>
   </si>
   <si>
-    <t>Home garden, young agroforest</t>
-  </si>
-  <si>
     <t>Yam, condiment </t>
   </si>
   <si>
@@ -184,6 +169,21 @@
   </si>
   <si>
     <t>Arenga, Corypha, Borassus</t>
+  </si>
+  <si>
+    <t>Silvopasture (SP)</t>
+  </si>
+  <si>
+    <t>SP (pasture, savanna or secondary forest), FG</t>
+  </si>
+  <si>
+    <t>CF,  SP (pasture, savanna or secondary forest), FG</t>
+  </si>
+  <si>
+    <t>CF, YA</t>
+  </si>
+  <si>
+    <t>HG, YA</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,141 +570,141 @@
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="325" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="200" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D4" s="1">
         <v>0.2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="237.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1">
         <v>0.3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1">
         <v>0.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>